<commit_message>
Optimized stack_functions.py and HFCBattACDesign_SH_260117.py
</commit_message>
<xml_diff>
--- a/app/ReqPowDATA.xlsx
+++ b/app/ReqPowDATA.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,299 +434,265 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>ReqPow_AC</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="B2" t="n">
+        <v>88.46433681225949</v>
+      </c>
+      <c r="C2" t="n">
+        <v>176.928673624519</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1102.084472680845</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1769.286736245189</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1769.286736245189</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1590.539972988636</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1590.539972988636</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1485.157928567575</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1485.157928567575</v>
+      </c>
+      <c r="K2" t="n">
+        <v>176.928673624519</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1769.286736245189</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1769.286736245189</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1485.157928567575</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1485.157928567575</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1485.157928567575</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>1485.157928567575</v>
+      </c>
+      <c r="R2" t="n">
+        <v>176.928673624519</v>
+      </c>
+      <c r="S2" t="n">
+        <v>176.928673624519</v>
+      </c>
+      <c r="T2" t="n">
+        <v>176.928673624519</v>
+      </c>
+      <c r="U2" t="n">
+        <v>88.46433681225949</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>ReqPow_FC</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="B3" t="n">
+        <v>88.46433681225949</v>
+      </c>
+      <c r="C3" t="n">
+        <v>176.928673624519</v>
+      </c>
+      <c r="D3" t="n">
+        <v>886.6166518988772</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1437.192219505459</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1437.192219505459</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1645.195671448263</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1645.195671448263</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1485.157928567575</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1485.157928567575</v>
+      </c>
+      <c r="K3" t="n">
+        <v>176.928673624519</v>
+      </c>
+      <c r="L3" t="n">
+        <v>1437.192219505459</v>
+      </c>
+      <c r="M3" t="n">
+        <v>1437.192219505459</v>
+      </c>
+      <c r="N3" t="n">
+        <v>1485.157928567575</v>
+      </c>
+      <c r="O3" t="n">
+        <v>1485.157928567575</v>
+      </c>
+      <c r="P3" t="n">
+        <v>1485.157928567575</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>1485.157928567575</v>
+      </c>
+      <c r="R3" t="n">
+        <v>176.928673624519</v>
+      </c>
+      <c r="S3" t="n">
+        <v>176.928673624519</v>
+      </c>
+      <c r="T3" t="n">
+        <v>176.928673624519</v>
+      </c>
+      <c r="U3" t="n">
+        <v>88.46433681225949</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>ReqPow_Batt</t>
         </is>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>88.46478119038883</v>
-      </c>
-      <c r="C2" t="n">
-        <v>88.46478119038883</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>176.9295623807777</v>
-      </c>
-      <c r="C3" t="n">
-        <v>176.9295623807777</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
       <c r="B4" t="n">
-        <v>1102.089876347605</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>886.6210818666552</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>215.4687944809496</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>1769.295623807777</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1437.199606333079</v>
-      </c>
-      <c r="D5" t="n">
-        <v>332.0960174746977</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>1769.295623807777</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1437.199606333079</v>
-      </c>
-      <c r="D6" t="n">
-        <v>332.0960174746977</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>1590.547993427122</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1645.203938875824</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-54.65594544870228</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>1590.547993427122</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1645.203938875824</v>
-      </c>
-      <c r="D8" t="n">
-        <v>-54.65594544870228</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1485.165391385093</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1485.165391385093</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1485.165391385093</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1485.165391385093</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>176.9295623807777</v>
-      </c>
-      <c r="C11" t="n">
-        <v>176.9295623807777</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1769.295623807777</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1437.199606333079</v>
-      </c>
-      <c r="D12" t="n">
-        <v>332.0960174746977</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="n">
-        <v>1769.295623807777</v>
-      </c>
-      <c r="C13" t="n">
-        <v>1437.199606333079</v>
-      </c>
-      <c r="D13" t="n">
-        <v>332.0960174746977</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="n">
-        <v>1485.165391385093</v>
-      </c>
-      <c r="C14" t="n">
-        <v>1485.165391385093</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="n">
-        <v>1485.165391385093</v>
-      </c>
-      <c r="C15" t="n">
-        <v>1485.165391385093</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="n">
-        <v>1485.165391385093</v>
-      </c>
-      <c r="C16" t="n">
-        <v>1485.165391385093</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="n">
-        <v>1485.165391385093</v>
-      </c>
-      <c r="C17" t="n">
-        <v>1485.165391385093</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="n">
-        <v>176.9295623807777</v>
-      </c>
-      <c r="C18" t="n">
-        <v>176.9295623807777</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="n">
-        <v>176.9295623807777</v>
-      </c>
-      <c r="C19" t="n">
-        <v>176.9295623807777</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="n">
-        <v>176.9295623807777</v>
-      </c>
-      <c r="C20" t="n">
-        <v>176.9295623807777</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="n">
-        <v>88.46478119038883</v>
-      </c>
-      <c r="C21" t="n">
-        <v>88.46478119038883</v>
-      </c>
-      <c r="D21" t="n">
+        <v>215.4678207819673</v>
+      </c>
+      <c r="E4" t="n">
+        <v>332.0945167397305</v>
+      </c>
+      <c r="F4" t="n">
+        <v>332.0945167397305</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-54.65569845962627</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-54.65569845962627</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>332.0945167397305</v>
+      </c>
+      <c r="M4" t="n">
+        <v>332.0945167397305</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>